<commit_message>
updated veg model parameters
</commit_message>
<xml_diff>
--- a/data/wwfeco.types.cover2.xlsx
+++ b/data/wwfeco.types.cover2.xlsx
@@ -3587,7 +3587,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K876" sqref="K876"/>
+      <selection pane="bottomLeft" activeCell="I329" sqref="I329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42996,7 +42996,7 @@
         <v>99</v>
       </c>
       <c r="H566">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I566">
         <v>10</v>
@@ -44348,7 +44348,7 @@
         <v>0</v>
       </c>
       <c r="G601">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="H601">
         <v>25</v>

</xml_diff>